<commit_message>
Get regression working. Start to sketch solver
</commit_message>
<xml_diff>
--- a/eval/notes.xlsx
+++ b/eval/notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/915f7bc53e120788/Projects/midi_tape_deck/eval/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmp\Documents\Max\midi_tape_deck\eval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{0182669E-04C6-408A-B35E-0A782B656239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D00DBBC-D64E-4EA8-AE0E-40608ECF7114}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F1CEF0-4FAC-42B3-A401-67E93D62CDC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C4C7B00-E495-47C8-AE3A-AB024DC55D7E}"/>
+    <workbookView xWindow="1635" yWindow="2460" windowWidth="21600" windowHeight="11385" xr2:uid="{0C4C7B00-E495-47C8-AE3A-AB024DC55D7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -620,17 +620,7 @@
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -655,6 +645,1148 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.12981450848055759"/>
+                  <c:y val="9.8395811636199759E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                      <a:t>y = 8.1757e</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1600" baseline="30000"/>
+                      <a:t>0.0578x</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                      <a:t>R² = 1</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1600"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$129</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="128"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>127</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$129</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="128"/>
+                <c:pt idx="0">
+                  <c:v>8.18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.66</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7200000000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.91</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.56</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.98</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.57</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.43</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17.32</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18.350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19.45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21.83</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23.12</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25.96</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>29.14</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>30.87</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>32.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>34.65</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>36.71</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>38.89</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41.2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43.65</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>46.25</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>51.91</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>58.27</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>61.74</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>65.41</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>69.3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>73.42</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>77.78</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>82.41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>87.31</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>103.83</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>116.54</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>123.47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>130.81</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>138.59</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>146.83000000000001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>155.56</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>164.81</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>174.61</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>207.65</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>233.08</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>246.94</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>261.63</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>277.18</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>293.66000000000003</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>311.13</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>329.63</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>349.23</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>369.99</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>392</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>415.3</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>466.16</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>493.88</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>523.25</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>554.37</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>587.33000000000004</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>622.25</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>659.25</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>698.46</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>739.99</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>783.99</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>830.61</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>932.33</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>987.77</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1046.5</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1108.73</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1174.6600000000001</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1244.51</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1318.51</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1396.91</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1479.98</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1567.98</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1661.22</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1760</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1864.66</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1975.53</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2093</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2217.46</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2349.3200000000002</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2489.02</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2637.02</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2793.83</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2959.96</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>3135.96</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>3322.44</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>3520</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>3729.31</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>3951.07</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>4186.01</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>4434.92</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>4698.63</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>4978.03</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>5274.04</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>5587.65</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>5919.91</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>6271.93</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>6644.88</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>7040</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>7458.62</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>7902.13</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>8372.02</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>8869.84</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>9397.27</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>9956.06</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>10548.08</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>11175.3</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>11839.82</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>12543.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AD7F-47C2-B51A-D524A8AFD6F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="580194440"/>
+        <c:axId val="451834368"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="580194440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="451834368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="451834368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="580194440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2653,6 +3785,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3208,6 +4380,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{49CF34BD-F895-47F1-A204-A816CA01B87B}">
   <sheetPr/>
@@ -3220,6 +4908,47 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>166686</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCE8B1E5-896A-4FFB-95C5-DFDE465E7AEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -3551,8 +5280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E877EEE3-EC07-4101-9E72-75741753E8A6}">
   <dimension ref="A1:H169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H109" sqref="H109"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" activeCellId="1" sqref="C2:C129 E2:E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5192,7 +6921,7 @@
         <v>2863.4424304899348</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G129" si="7">E68-E67</f>
+        <f t="shared" ref="G67:G128" si="7">E68-E67</f>
         <v>20.759999999999991</v>
       </c>
       <c r="H67">
@@ -5482,7 +7211,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="13"/>
       <c r="B78" s="5" t="s">
         <v>80</v>
@@ -7342,5 +9071,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>